<commit_message>
trace length matching & generate gerber files
</commit_message>
<xml_diff>
--- a/doc/trace-length.xlsx
+++ b/doc/trace-length.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\FlightComputer\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Private\src\FlightComputer_\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFE0149-6E89-40A2-A1C3-24C4E5E175D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B846102-C97E-4763-A522-04E28FB37FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="90" windowWidth="26175" windowHeight="15810" xr2:uid="{0F001A9B-73FB-4382-A976-C7CA4EDAAC36}"/>
+    <workbookView xWindow="28950" yWindow="285" windowWidth="13290" windowHeight="15075" xr2:uid="{0F001A9B-73FB-4382-A976-C7CA4EDAAC36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>NOR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,10 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BA2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BL0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -217,6 +213,22 @@
   </si>
   <si>
     <t>AVG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Via 0.45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BA0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -224,7 +236,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,7 +302,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -301,6 +316,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,15 +635,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D423195-2BA0-4C1F-A626-6B50C7808596}">
-  <dimension ref="C4:I50"/>
+  <dimension ref="C4:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -633,32 +654,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10">
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
-        <v>47</v>
+      <c r="E5" t="s">
+        <v>51</v>
       </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
       </c>
       <c r="I5">
         <v>80.938000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
         <v>74.808999999999997</v>
       </c>
+      <c r="E6">
+        <v>75</v>
+      </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="H6">
         <v>49.091999999999999</v>
@@ -666,16 +696,22 @@
       <c r="I6" s="4">
         <v>80.935000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7">
         <v>74.751999999999995</v>
       </c>
+      <c r="E7">
+        <v>74.84</v>
+      </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <v>48.722999999999999</v>
@@ -683,16 +719,22 @@
       <c r="I7" s="4">
         <v>80.97</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8">
         <v>74.744</v>
       </c>
+      <c r="E8">
+        <v>75.018000000000001</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2">
         <v>80.653000000000006</v>
@@ -700,16 +742,22 @@
       <c r="I8" s="4">
         <v>80.923000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9">
         <v>74.516000000000005</v>
       </c>
+      <c r="E9">
+        <v>74.986000000000004</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2">
         <v>72.188999999999993</v>
@@ -717,16 +765,22 @@
       <c r="I9" s="4">
         <v>80.864000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10">
         <v>74.7</v>
       </c>
+      <c r="E10">
+        <v>74.998999999999995</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10">
         <v>67.227999999999994</v>
@@ -734,14 +788,20 @@
       <c r="I10" s="4">
         <v>80.867000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
         <v>74.7</v>
       </c>
+      <c r="E11">
+        <v>75</v>
+      </c>
       <c r="G11" t="s">
         <v>1</v>
       </c>
@@ -751,10 +811,13 @@
       <c r="I11" s="4">
         <v>80.831999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12">
         <v>75.016000000000005</v>
@@ -762,10 +825,13 @@
       <c r="I12" s="4">
         <v>80.843999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13">
         <v>69.471000000000004</v>
@@ -773,17 +839,24 @@
       <c r="I13" s="4">
         <v>80.897999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <f>AVERAGE(D6:D11)</f>
         <v>74.703499999999991</v>
       </c>
+      <c r="E14">
+        <f>AVERAGE(E6:E11)</f>
+        <v>74.973833333333332</v>
+      </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14">
         <v>80.938000000000002</v>
@@ -791,17 +864,24 @@
       <c r="I14" s="4">
         <v>80.938000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15">
         <f>MIN(D6:D11)</f>
         <v>74.516000000000005</v>
       </c>
+      <c r="E15">
+        <f>MIN(E6:E11)</f>
+        <v>74.84</v>
+      </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <v>79.518000000000001</v>
@@ -809,17 +889,24 @@
       <c r="I15" s="4">
         <v>80.814999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <f>MAX(D6:D11)</f>
         <v>74.808999999999997</v>
       </c>
+      <c r="E16">
+        <f>MAX(E6:E11)</f>
+        <v>75.018000000000001</v>
+      </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16">
         <v>69.695999999999998</v>
@@ -827,17 +914,24 @@
       <c r="I16" s="4">
         <v>80.948999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <f>D16-D15</f>
         <v>0.29299999999999216</v>
       </c>
+      <c r="E17">
+        <f>E16-E15</f>
+        <v>0.17799999999999727</v>
+      </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17">
         <v>49.344999999999999</v>
@@ -845,10 +939,13 @@
       <c r="I17" s="4">
         <v>80.835999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>82.242000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10">
       <c r="G18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18">
         <v>49.478999999999999</v>
@@ -856,10 +953,13 @@
       <c r="I18" s="4">
         <v>80.837999999999994</v>
       </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10">
       <c r="G19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19">
         <v>43.366999999999997</v>
@@ -867,10 +967,13 @@
       <c r="I19" s="4">
         <v>80.897999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10">
       <c r="G20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20">
         <v>62.039000000000001</v>
@@ -878,10 +981,13 @@
       <c r="I20" s="4">
         <v>80.888999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10">
       <c r="G21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21">
         <v>48.6</v>
@@ -889,10 +995,13 @@
       <c r="I21" s="4">
         <v>80.834000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10">
       <c r="G22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22">
         <v>50.597999999999999</v>
@@ -900,10 +1009,13 @@
       <c r="I22" s="4">
         <v>80.888000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10">
       <c r="G23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H23">
         <v>53.524000000000001</v>
@@ -911,10 +1023,13 @@
       <c r="I23" s="4">
         <v>80.753</v>
       </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
       <c r="G24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H24">
         <v>56.755000000000003</v>
@@ -922,10 +1037,13 @@
       <c r="I24" s="4">
         <v>80.813999999999993</v>
       </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10">
       <c r="G25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25">
         <v>74.968999999999994</v>
@@ -933,10 +1051,16 @@
       <c r="I25" s="4">
         <v>80.924999999999997</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10">
+      <c r="D26">
+        <v>80.971000000000004</v>
+      </c>
       <c r="G26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26">
         <v>76.671000000000006</v>
@@ -944,10 +1068,16 @@
       <c r="I26" s="4">
         <v>80.947000000000003</v>
       </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10">
+      <c r="D27">
+        <v>80.207999999999998</v>
+      </c>
       <c r="G27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27">
         <v>76.945999999999998</v>
@@ -955,8 +1085,15 @@
       <c r="I27" s="4">
         <v>80.796000000000006</v>
       </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="D28">
+        <f>D26-D27</f>
+        <v>0.76300000000000523</v>
+      </c>
       <c r="G28" t="s">
         <v>8</v>
       </c>
@@ -966,8 +1103,15 @@
       <c r="I28" s="4">
         <v>80.914000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="D29">
+        <f>82.241-D28</f>
+        <v>81.477999999999994</v>
+      </c>
       <c r="G29" t="s">
         <v>9</v>
       </c>
@@ -977,8 +1121,11 @@
       <c r="I29" s="4">
         <v>80.957999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
       <c r="G30" t="s">
         <v>10</v>
       </c>
@@ -988,8 +1135,11 @@
       <c r="I30" s="4">
         <v>80.900000000000006</v>
       </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10">
       <c r="G31" t="s">
         <v>11</v>
       </c>
@@ -999,8 +1149,11 @@
       <c r="I31" s="4">
         <v>80.962000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
       <c r="G32" t="s">
         <v>12</v>
       </c>
@@ -1010,8 +1163,11 @@
       <c r="I32" s="4">
         <v>80.998000000000005</v>
       </c>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10">
       <c r="G33" t="s">
         <v>13</v>
       </c>
@@ -1021,8 +1177,11 @@
       <c r="I33" s="4">
         <v>80.757999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10">
       <c r="G34" t="s">
         <v>14</v>
       </c>
@@ -1032,8 +1191,11 @@
       <c r="I34" s="4">
         <v>80.823999999999998</v>
       </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10">
       <c r="G35" t="s">
         <v>15</v>
       </c>
@@ -1043,8 +1205,11 @@
       <c r="I35" s="4">
         <v>80.731999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10">
       <c r="G36" t="s">
         <v>16</v>
       </c>
@@ -1054,8 +1219,11 @@
       <c r="I36" s="4">
         <v>80.747</v>
       </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10">
       <c r="G37" t="s">
         <v>17</v>
       </c>
@@ -1065,8 +1233,11 @@
       <c r="I37" s="4">
         <v>80.646000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10">
       <c r="G38" t="s">
         <v>18</v>
       </c>
@@ -1076,8 +1247,11 @@
       <c r="I38" s="4">
         <v>80.97</v>
       </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10">
       <c r="G39" t="s">
         <v>19</v>
       </c>
@@ -1087,10 +1261,13 @@
       <c r="I39" s="4">
         <v>80.971999999999994</v>
       </c>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10">
       <c r="G40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H40">
         <v>60.753999999999998</v>
@@ -1098,10 +1275,13 @@
       <c r="I40" s="4">
         <v>80.850999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10">
       <c r="G41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H41">
         <v>80.039000000000001</v>
@@ -1109,10 +1289,13 @@
       <c r="I41" s="4">
         <v>80.799000000000007</v>
       </c>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10">
       <c r="G42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H42">
         <v>72.638000000000005</v>
@@ -1120,10 +1303,13 @@
       <c r="I42" s="4">
         <v>80.959999999999994</v>
       </c>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10">
       <c r="G43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H43">
         <v>48.29</v>
@@ -1131,10 +1317,13 @@
       <c r="I43" s="4">
         <v>80.753</v>
       </c>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10">
       <c r="G44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H44">
         <v>64.341999999999999</v>
@@ -1142,29 +1331,60 @@
       <c r="I44" s="4">
         <v>80.92</v>
       </c>
-    </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10">
       <c r="H47" t="s">
         <v>48</v>
       </c>
       <c r="I47">
+        <f>MAX(I6:I44)</f>
+        <v>80.998000000000005</v>
+      </c>
+      <c r="J47">
+        <f>MAX(J6:J44)</f>
+        <v>82.242000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10">
+      <c r="H48" t="s">
+        <v>47</v>
+      </c>
+      <c r="I48">
         <f>MIN(I6:I44)</f>
         <v>80.646000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="H48" t="s">
-        <v>49</v>
-      </c>
-      <c r="I48">
-        <f>MAX(I6:I44)</f>
-        <v>80.998000000000005</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50">
-        <f>I48-I47</f>
+      <c r="J48">
+        <f>MIN(J6:J44)</f>
+        <v>82.241</v>
+      </c>
+    </row>
+    <row r="49" spans="8:10">
+      <c r="H49" t="s">
+        <v>52</v>
+      </c>
+      <c r="I49" s="5">
+        <f>AVERAGE(I6:I44)</f>
+        <v>80.869666666666674</v>
+      </c>
+      <c r="J49" s="5">
+        <f>AVERAGE(J6:J44)</f>
+        <v>82.24102564102563</v>
+      </c>
+    </row>
+    <row r="51" spans="8:10">
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51">
+        <f>I47-I48</f>
         <v>0.35200000000000387</v>
+      </c>
+      <c r="J51">
+        <f>J47-J48</f>
+        <v>1.0000000000047748E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>